<commit_message>
Bento QA test suite in Jenkins 11 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_E2E_Select-All-Add-To-Cart.xlsx
+++ b/InputFiles/TC01_Bento_E2E_Select-All-Add-To-Cart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB16C2BE-F198-4335-AA07-98F60731A5C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A006808C-E8C3-4555-B938-F258624966B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>dbExcel</t>
   </si>
   <si>
-    <t>TC01_Bento_E2E_Select-All-Add-To-Cart_Neo4jData.xlsx</t>
-  </si>
-  <si>
     <t>TC01_Bento_E2E_Select-All-Add-To-Cart_WebData.xlsx</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve"> https://qa.bento-tools.org/</t>
+  </si>
+  <si>
+    <t>TC01_Bento_E2E_Select-All-Add-To-Cart_Manifest.csv</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -485,16 +485,16 @@
     </row>
     <row r="2" spans="1:4" ht="377" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
e2e single case addition, bento perf ts
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_E2E_Select-All-Add-To-Cart.xlsx
+++ b/InputFiles/TC01_Bento_E2E_Select-All-Add-To-Cart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B745CC-3ACC-4F3A-8A6E-F9759F482370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F47A475-CC0D-4283-9899-B5A4F76616C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -51,6 +51,9 @@
     <t xml:space="preserve"> https://qa.bento-tools.org/</t>
   </si>
   <si>
+    <t>TC01_Bento_E2E_Select-All-Add-To-Cart_Manifest.xlsx</t>
+  </si>
+  <si>
     <t>MATCH (ss:study_subject)
 MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(samp:sample)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
@@ -60,7 +63,7 @@
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
 MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE ss.disease_subtype IN ["Tubular Carcinoma"] and d.tumor_size_group In ["(3,4]"] and d.er_status In ["Positive"]and d.pr_status In ["Positive"] and tp.endocrine_therapy_type IN ["Other"]  and head(labels(samp)) IN ["sample"]
+WHERE ss.disease_subtype IN ["Tubular Carcinoma"] and d.tumor_size_group In ["(3,4]"] and d.er_status In ["Positive"]and d.pr_status In ["Positive"]  
 return DISTINCT ss.study_subject_id as `Case ID`,
    p.program_acronym as `Program Code`,
     p.program_id as Program_ID,
@@ -72,9 +75,6 @@
    d.pr_status AS `PR Status`,
    demo.age_at_index AS `Age (years)`,
 	demo.survival_time AS `Survival (days)`</t>
-  </si>
-  <si>
-    <t>TC01_Bento_E2E_Select-All-Add-To-Cart_Manifest.xlsx</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,15 +483,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="390" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="375" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>

</xml_diff>